<commit_message>
BIG update: several changes and WIP experimentations
</commit_message>
<xml_diff>
--- a/Ruter/Antall påstigende per dag_Oslo_2015_2017.xlsx
+++ b/Ruter/Antall påstigende per dag_Oslo_2015_2017.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\80_Kvalitet og prosjekt\Analyse\Analyse_Leveranser\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36090" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Antall påstigende per dag_Oslo" sheetId="2" r:id="rId1"/>
@@ -3552,10 +3547,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -3596,10 +3591,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3904,7 +3899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3918,7 +3913,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>